<commit_message>
Update data and data prep notebook
</commit_message>
<xml_diff>
--- a/data/arte-urbana-manual.xlsx
+++ b/data/arte-urbana-manual.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joao.palmeiro/Documents/GitHub/amadora-arte-urbana/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD07D1CE-B71A-644F-9095-57B0D00EC504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA7CA911-56F1-5E4C-93C5-0EF7CECB45B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16140" xr2:uid="{993D80B6-E727-4A50-A805-B4D13277D6CE}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="455">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="996" uniqueCount="468">
   <si>
     <t>ID</t>
   </si>
@@ -1411,6 +1411,49 @@
   </si>
   <si>
     <t>Raps, Vespa, Sken, New, Styler, 1ma63, Creyz, Vile, Rote, Odeith, Eko e Molin</t>
+  </si>
+  <si>
+    <t>«Era mais influenciado pelo que vivia no dia-a-dia.»
+Mural localizado no Bairro da Cova da Moura, na freguesia da Damaia. Exibe uma figura mediática e vista como um exemplo na comunidade, o intérprete Bob Marley.</t>
+  </si>
+  <si>
+    <t>«A expressão graffiti vem da expressão “getting up”, que é tu levantares o teu nome, seres alguém, seres reconhecido na terra onde vives.»
+Mural localizado no Bairro da Cova da Moura, na freguesia da Damaia e que presta homenagem ao jogador de futebol Eusébio.</t>
+  </si>
+  <si>
+    <t>«Este é um dos meus murais preferidos. Sempre fui um frequentador do festival Amadora BD e sou muito influenciado pela banda desenhada. Este mural foi o primeiro no qual desenvolvi um estilo que ainda não tinha transportado para uma parede.»</t>
+  </si>
+  <si>
+    <t>Mural realizado no âmbito do Concurso de Pintura de Murais sobre Banda Desenhada, promovido pelas Estradas de Portugal e em parceria com a Câmara Municipal da Amadora.</t>
+  </si>
+  <si>
+    <t>Mural localizado nas traseiras da Escola Secundária D. João V, na Damaia. Este mural representa uma homenagem aos bombeiros, vítimas dos incêndios.</t>
+  </si>
+  <si>
+    <t>Mural localizado nas traseiras da Escola Secundária D. João V, na Damaia.</t>
+  </si>
+  <si>
+    <t>Mural localizado nas traseiras da Escola Secundária D. João V, na Damaia. Odeith colaborou com a artista urbana argentina Milu Correch na realização deste mural.</t>
+  </si>
+  <si>
+    <t>«[O graffiti] é uma manifestação e se tu vires acho que nas zonas com mais população, ou seja, onde há prédios maiores, onde há se calhar guetos é onde as pessoas se tendem a manifestar e arriscar, e isso sempre foi assim e há-de ser.»
+Mural localizado nas traseiras da Escola Secundária D. João V, na Damaia.</t>
+  </si>
+  <si>
+    <t>Hall of Fame localizado nas traseiras da Escola Secundária D. João V, na Damaia.</t>
+  </si>
+  <si>
+    <t>Eko, membro da GVS Crew: «O meu interesse surgiu no ano de 1997, ano esse que se assistia a um grande boom da cultura hip-hop, desse boom surgem muitas crews e muitos writers. Eu fui um deles, surjo no seio de uma das crews mais antigas de Portugal, GVS, que ainda está activa, com writers espalhados por todo o mundo.»</t>
+  </si>
+  <si>
+    <t>«Comecei a pintar em 1989. Para mim o Graffiti é estares artilhado de formas, de contextos para poderes singrar na vida.»</t>
+  </si>
+  <si>
+    <t>«O meu interesse pelo Graffiti surgiu porque os meus primos ouviam rap, desenhavam nas calças de ganga e eu imitava. Depois segui para as paredes.»
+Mural realizado e que presta homenagem ao artista urbano Broke.</t>
+  </si>
+  <si>
+    <t>Peça realizada no âmbito do Concurso de Pintura de Murais sobre Banda Desenhada, promovido pelas Estradas de Portugal e em parceria com a Câmara Municipal da Amadora.</t>
   </si>
 </sst>
 </file>
@@ -1851,9 +1894,9 @@
   <dimension ref="A1:M138"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="L1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="M14" sqref="M14"/>
+      <selection pane="bottomLeft" activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1868,7 +1911,8 @@
     <col min="8" max="8" width="71.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="100.83203125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="100.83203125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="125.83203125" style="2" customWidth="1"/>
     <col min="13" max="13" width="50.83203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1951,7 +1995,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>3</v>
       </c>
@@ -1984,6 +2028,9 @@
       </c>
       <c r="K3" s="3" t="s">
         <v>21</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>455</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="48" x14ac:dyDescent="0.2">
@@ -2020,6 +2067,9 @@
       <c r="K4" s="3" t="s">
         <v>24</v>
       </c>
+      <c r="L4" s="3" t="s">
+        <v>456</v>
+      </c>
     </row>
     <row r="5" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A5">
@@ -2055,6 +2105,9 @@
       <c r="K5" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="L5" s="3" t="s">
+        <v>457</v>
+      </c>
     </row>
     <row r="6" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A6">
@@ -2090,6 +2143,9 @@
       <c r="K6" s="3" t="s">
         <v>34</v>
       </c>
+      <c r="L6" s="3" t="s">
+        <v>458</v>
+      </c>
     </row>
     <row r="7" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A7">
@@ -2125,6 +2181,9 @@
       <c r="K7" s="3" t="s">
         <v>39</v>
       </c>
+      <c r="L7" s="2" t="s">
+        <v>459</v>
+      </c>
     </row>
     <row r="8" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -2160,6 +2219,9 @@
       <c r="K8" s="3" t="s">
         <v>41</v>
       </c>
+      <c r="L8" s="3" t="s">
+        <v>460</v>
+      </c>
     </row>
     <row r="9" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A9">
@@ -2195,6 +2257,9 @@
       <c r="K9" s="3" t="s">
         <v>44</v>
       </c>
+      <c r="L9" s="2" t="s">
+        <v>461</v>
+      </c>
     </row>
     <row r="10" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A10">
@@ -2230,6 +2295,9 @@
       <c r="K10" s="3" t="s">
         <v>48</v>
       </c>
+      <c r="L10" s="2" t="s">
+        <v>462</v>
+      </c>
     </row>
     <row r="11" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A11">
@@ -2265,6 +2333,9 @@
       <c r="K11" s="3" t="s">
         <v>51</v>
       </c>
+      <c r="L11" s="3" t="s">
+        <v>460</v>
+      </c>
     </row>
     <row r="12" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A12">
@@ -2296,6 +2367,9 @@
       </c>
       <c r="K12" s="3" t="s">
         <v>53</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>460</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="32" x14ac:dyDescent="0.2">
@@ -2332,6 +2406,9 @@
       <c r="K13" s="3" t="s">
         <v>57</v>
       </c>
+      <c r="L13" s="3" t="s">
+        <v>463</v>
+      </c>
       <c r="M13" s="2" t="s">
         <v>454</v>
       </c>
@@ -2370,6 +2447,9 @@
       <c r="K14" s="3" t="s">
         <v>60</v>
       </c>
+      <c r="L14" s="2" t="s">
+        <v>464</v>
+      </c>
     </row>
     <row r="15" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A15">
@@ -2405,6 +2485,9 @@
       <c r="K15" s="3" t="s">
         <v>63</v>
       </c>
+      <c r="L15" s="3" t="s">
+        <v>458</v>
+      </c>
     </row>
     <row r="16" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A16">
@@ -2440,8 +2523,11 @@
       <c r="K16" s="3" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="L16" s="3" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>9</v>
       </c>
@@ -2475,8 +2561,11 @@
       <c r="K17" s="3" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="L17" s="2" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>10</v>
       </c>
@@ -2510,8 +2599,11 @@
       <c r="K18" s="3" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="L18" s="3" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>11</v>
       </c>
@@ -2545,8 +2637,11 @@
       <c r="K19" s="3" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="L19" s="3" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>6</v>
       </c>
@@ -2580,8 +2675,11 @@
       <c r="K20" s="3" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="L20" s="3" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>33</v>
       </c>
@@ -2615,8 +2713,11 @@
       <c r="K21" s="3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="L21" s="3" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>34</v>
       </c>
@@ -2650,8 +2751,11 @@
       <c r="K22" s="3" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="L22" s="2" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>12</v>
       </c>
@@ -2685,8 +2789,11 @@
       <c r="K23" s="3" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="L23" s="3" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>13</v>
       </c>
@@ -2721,7 +2828,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>14</v>
       </c>
@@ -2756,7 +2863,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>15</v>
       </c>
@@ -2791,7 +2898,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>16</v>
       </c>
@@ -2826,7 +2933,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>17</v>
       </c>
@@ -2861,7 +2968,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>18</v>
       </c>
@@ -2896,7 +3003,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>19</v>
       </c>
@@ -2931,7 +3038,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>20</v>
       </c>
@@ -2966,7 +3073,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>21</v>
       </c>

</xml_diff>